<commit_message>
commiting stuff from home
</commit_message>
<xml_diff>
--- a/Spreadsheets/trai_norm_email_features_100_0 (2).xlsx
+++ b/Spreadsheets/trai_norm_email_features_100_0 (2).xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="trai_norm_email_features_100_0 " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>